<commit_message>
New Staging Branch Signed-off-by: ffpoke <aleard1@proton.me>
</commit_message>
<xml_diff>
--- a/3.x/3.0.xlsx
+++ b/3.x/3.0.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marink\Documents\FFXIV Excel\3.x\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marink\Documents\FFXIV-EXCEL\3.x\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254C167B-60D5-4484-B694-094464127D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60E9153-2F90-4B15-97CF-6109EE44C5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="7845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3.0" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="3.0 MSQ" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -48,9 +48,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Havensward (3.0)</t>
+  </si>
+  <si>
+    <t>Main Story Quest</t>
   </si>
 </sst>
 </file>
@@ -66,6 +69,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri Light"/>
@@ -447,9 +451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F1D066-DCA9-470F-BD04-154644ED5331}">
   <dimension ref="B1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:J2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -480,6 +482,11 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
@@ -608,9 +615,10 @@
       <c r="E24" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:E24"/>
     <mergeCell ref="F1:J2"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -620,7 +628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Level 50-51 MSQ Signed-off-by: ffpoke <aleard1@proton.me>
</commit_message>
<xml_diff>
--- a/3.x/3.0.xlsx
+++ b/3.x/3.0.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marink\Documents\FFXIV-EXCEL\3.x\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60E9153-2F90-4B15-97CF-6109EE44C5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F4DFF1-31A8-4BBC-BF5E-95A050B6B5F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="739" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3.0" sheetId="2" r:id="rId1"/>
-    <sheet name="3.0 MSQ" sheetId="1" r:id="rId2"/>
+    <sheet name="Havensward MSQ" sheetId="3" r:id="rId2"/>
+    <sheet name="3.0 MSQ &amp; Artoirel Quests" sheetId="1" r:id="rId3"/>
+    <sheet name="Emmanellain Quests" sheetId="4" r:id="rId4"/>
+    <sheet name="3.0 MSQ Cont." sheetId="5" r:id="rId5"/>
+    <sheet name="Levels 52-53" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -48,19 +52,151 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>Havensward (3.0)</t>
   </si>
   <si>
     <t>Main Story Quest</t>
+  </si>
+  <si>
+    <t>Quests</t>
+  </si>
+  <si>
+    <t>Havensward MSQ</t>
+  </si>
+  <si>
+    <t>Levels 58-60</t>
+  </si>
+  <si>
+    <t>Levels 56-57</t>
+  </si>
+  <si>
+    <t>Levels 54-55</t>
+  </si>
+  <si>
+    <t>Levels 52-53</t>
+  </si>
+  <si>
+    <t>Emmanellain Quest</t>
+  </si>
+  <si>
+    <t>Artoirel Quests</t>
+  </si>
+  <si>
+    <t>Main Story Quest (Continued)</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Coming to Ishgard</t>
+  </si>
+  <si>
+    <t>Taking in the Sights</t>
+  </si>
+  <si>
+    <t>The Better Half</t>
+  </si>
+  <si>
+    <t>Main Story Quests</t>
+  </si>
+  <si>
+    <t>Over the Wall</t>
+  </si>
+  <si>
+    <t>Work in Progress</t>
+  </si>
+  <si>
+    <t>The First and Foremost</t>
+  </si>
+  <si>
+    <t>From on High</t>
+  </si>
+  <si>
+    <t>Reconnaissance Lost</t>
+  </si>
+  <si>
+    <t>At the End of Our Hope</t>
+  </si>
+  <si>
+    <t>Knights Be Not Proud</t>
+  </si>
+  <si>
+    <t>Emmanellain Story Quests</t>
+  </si>
+  <si>
+    <t>Artoirel Story Quests</t>
+  </si>
+  <si>
+    <t>Main Story Quests Continued</t>
+  </si>
+  <si>
+    <t>Onwards and Upwards</t>
+  </si>
+  <si>
+    <t>An Indispensable Ally</t>
+  </si>
+  <si>
+    <t>Meeting the Neighbors</t>
+  </si>
+  <si>
+    <t>Sense of Urgency</t>
+  </si>
+  <si>
+    <t>Hope Springs Eternal</t>
+  </si>
+  <si>
+    <t>A Series of Unfortunate Events</t>
+  </si>
+  <si>
+    <t>A Reward Long in Coming</t>
+  </si>
+  <si>
+    <t>Divine Intervention</t>
+  </si>
+  <si>
+    <t>Disclosure</t>
+  </si>
+  <si>
+    <t>Flame General Affairs</t>
+  </si>
+  <si>
+    <t>In Search of Raubahn</t>
+  </si>
+  <si>
+    <t>Keeping the Flame Alive</t>
+  </si>
+  <si>
+    <t>To Siege or Not to Siege</t>
+  </si>
+  <si>
+    <t>Alphinaud's Way</t>
+  </si>
+  <si>
+    <t>In Search of Iceheart</t>
+  </si>
+  <si>
+    <t>From One Heretic to Another</t>
+  </si>
+  <si>
+    <t>Sounding Out the Amphitheatre</t>
+  </si>
+  <si>
+    <t>Camp of the Convictors</t>
+  </si>
+  <si>
+    <t>Purple Flame, Purple Flame</t>
+  </si>
+  <si>
+    <t>Levels 52-53 Quests</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +207,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri Light"/>
       <family val="2"/>
@@ -97,13 +241,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -120,6 +294,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/featurePropertyBag/featurePropertyBag.xml><?xml version="1.0" encoding="utf-8"?>
+<FeaturePropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag">
+  <bag type="Checkbox"/>
+  <bag type="XFControls">
+    <bagId k="CellControl">0</bagId>
+  </bag>
+  <bag type="XFComplement">
+    <bagId k="XFControls">1</bagId>
+  </bag>
+  <bag type="XFComplements" extRef="XFComplementsMapperExtRef">
+    <a k="MappedFeaturePropertyBags">
+      <bagId>2</bagId>
+    </a>
+  </bag>
+</FeaturePropertyBags>
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
@@ -625,13 +816,762 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F51703-6368-459D-8255-6B7F733BBDCF}">
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7:D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B5:D5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="A7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB7E50A3-6ED5-4436-BE6E-FE1C7C6BEFFD}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="B8:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="A8:A9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F8CF94-EFCB-4834-A7F1-94693B5C3FDD}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B12:D13"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B7:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64108C3F-49EA-4963-A2EC-B8B11C344CAE}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="E1:E2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>